<commit_message>
Complete 8.3 Solo Challenge: Build a Database.
</commit_message>
<xml_diff>
--- a/databases/solo_project/solo_project_schema.xlsx
+++ b/databases/solo_project/solo_project_schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,8 +407,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -521,8 +521,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -635,8 +635,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -749,8 +749,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -863,8 +863,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -977,8 +977,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -1091,8 +1091,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1205,8 +1205,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1319,8 +1319,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1433,8 +1433,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1547,8 +1547,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1661,8 +1661,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1775,8 +1775,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1889,8 +1889,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2003,8 +2003,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2117,8 +2117,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2231,8 +2231,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2345,8 +2345,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2459,8 +2459,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2573,8 +2573,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2687,8 +2687,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2801,8 +2801,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -2915,8 +2915,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3029,8 +3029,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3143,8 +3143,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3257,8 +3257,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3371,8 +3371,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3485,8 +3485,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3599,8 +3599,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3713,8 +3713,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3827,8 +3827,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3884,8 +3884,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
@@ -3941,8 +3941,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3998,8 +3998,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4055,8 +4055,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4112,8 +4112,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4169,8 +4169,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4226,8 +4226,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4283,8 +4283,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4340,8 +4340,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4397,8 +4397,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4454,8 +4454,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -5048,14 +5048,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="3" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="7" width="3" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -5101,8 +5106,8 @@
         <v>83</v>
       </c>
       <c r="J2" t="str">
-        <f>CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2)</f>
-        <v>American Theocracy: The Peril and Politics of Radical Religion, Oil and Borrowed Money in the 21st Century","Phillips, Kevin",3.85,39461),</v>
+        <f>CONCATENATE(A2, B2,C2,D2,E2,F2,G2,H2,I2)</f>
+        <v>("American Theocracy: The Peril and Politics of Radical Religion, Oil and Borrowed Money in the 21st Century","Phillips, Kevin",3.85,39461),</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5134,8 +5139,8 @@
         <v>83</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J30" si="0">CONCATENATE(B3,C3,D3,E3,F3,G3,H3,I3)</f>
-        <v>Amusing Ourselves to Death: Public Discourse in the Age of Show Business","Postman, Neil",4.11,39453),</v>
+        <f t="shared" ref="J3:J30" si="0">CONCATENATE(A3, B3,C3,D3,E3,F3,G3,H3,I3)</f>
+        <v>("Amusing Ourselves to Death: Public Discourse in the Age of Show Business","Postman, Neil",4.11,39453),</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5168,7 +5173,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>Angry Black White Boy","Mansbach, Adam *",3.53,39453),</v>
+        <v>("Angry Black White Boy","Mansbach, Adam *",3.53,39453),</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5201,7 +5206,7 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>Arms and the Man","Shaw, George Bernard",3.84,39696),</v>
+        <v>("Arms and the Man","Shaw, George Bernard",3.84,39696),</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5234,7 +5239,7 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>As I Am: Young African American Women in a Critical Age","Okwu, Julian C.R.",4.29,39757),</v>
+        <v>("As I Am: Young African American Women in a Critical Age","Okwu, Julian C.R.",4.29,39757),</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5267,7 +5272,7 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>Boom! Voices of the Sixties Personal Reflections on the '60s and Today","Brokaw, Tom",3.75,39724),</v>
+        <v>("Boom! Voices of the Sixties Personal Reflections on the '60s and Today","Brokaw, Tom",3.75,39724),</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5300,7 +5305,7 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>Built to Last: Successful Habits of Visionary Companies","Collins, James C.",3.95,39766),</v>
+        <v>("Built to Last: Successful Habits of Visionary Companies","Collins, James C.",3.95,39766),</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5333,7 +5338,7 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>Extremely Loud and Incredibly Close","Safran Foer, Jonathan",3.97,39445),</v>
+        <v>("Extremely Loud and Incredibly Close","Safran Foer, Jonathan",3.97,39445),</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5366,7 +5371,7 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>Full Frontal Feminism","Valenti, Jessica *",3.85,39453),</v>
+        <v>("Full Frontal Feminism","Valenti, Jessica *",3.85,39453),</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5399,7 +5404,7 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>Games for Actors and Non-Actors","Boal, Augusto",4.35,39453),</v>
+        <v>("Games for Actors and Non-Actors","Boal, Augusto",4.35,39453),</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5432,7 +5437,7 @@
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
-        <v>Here Comes Everybody: The Power of Organizing Without Organizations","Shirky, Clay",3.82,39959),</v>
+        <v>("Here Comes Everybody: The Power of Organizing Without Organizations","Shirky, Clay",3.82,39959),</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5465,7 +5470,7 @@
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
-        <v>Lying Awake","Salzman, Mark",3.8,39603),</v>
+        <v>("Lying Awake","Salzman, Mark",3.8,39603),</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5498,7 +5503,7 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
-        <v>Mountains Beyond Mountains: The Quest of Dr. Paul Farmer, A Man Who Would Cure the World","Kidder, Tracy",4.2,39489),</v>
+        <v>("Mountains Beyond Mountains: The Quest of Dr. Paul Farmer, A Man Who Would Cure the World","Kidder, Tracy",4.2,39489),</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5531,7 +5536,7 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>No Country For Old Men","McCarthy, Cormac",4.12,39467),</v>
+        <v>("No Country For Old Men","McCarthy, Cormac",4.12,39467),</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5564,7 +5569,7 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>Oh Pure and Radiant Heart","Millet, Lydia",3.67,39489),</v>
+        <v>("Oh Pure and Radiant Heart","Millet, Lydia",3.67,39489),</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5597,7 +5602,7 @@
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>Predictably Irrational: The Hidden Forces That Shape Our Decisions","Ariely, Dan",4.08,39973),</v>
+        <v>("Predictably Irrational: The Hidden Forces That Shape Our Decisions","Ariely, Dan",4.08,39973),</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5630,7 +5635,7 @@
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
-        <v>Ten Little Indians","Alexie, Sherman",4.08,39392),</v>
+        <v>("Ten Little Indians","Alexie, Sherman",4.08,39392),</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5663,7 +5668,7 @@
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>The Audacity of Hope: Thoughts on Reclaiming the American Dream","Obama, Barack",3.67,39542),</v>
+        <v>("The Audacity of Hope: Thoughts on Reclaiming the American Dream","Obama, Barack",3.67,39542),</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5696,7 +5701,7 @@
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>The Bottom Billion: Why the Poorest Countries Are Failing and What Can Be Done About It","Collier, Paul",3.83,39563),</v>
+        <v>("The Bottom Billion: Why the Poorest Countries Are Failing and What Can Be Done About It","Collier, Paul",3.83,39563),</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5729,7 +5734,7 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>The Cluetrain Manifesto","Levine, Rick",3.86,39959),</v>
+        <v>("The Cluetrain Manifesto","Levine, Rick",3.86,39959),</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5762,7 +5767,7 @@
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>The Color of Water: A Black Man's Tribute to His White Mother","McBride, James *",4.05,39717),</v>
+        <v>("The Color of Water: A Black Man's Tribute to His White Mother","McBride, James *",4.05,39717),</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5795,7 +5800,7 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>The Fortune at the Bottom of the Pyramid: Eradicating Poverty Through Profits","Prahalad, C.K.",3.86,39563),</v>
+        <v>("The Fortune at the Bottom of the Pyramid: Eradicating Poverty Through Profits","Prahalad, C.K.",3.86,39563),</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5828,7 +5833,7 @@
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>The Practical Progressive: How to Build a Twenty-first Century Political Movement","Payne, Erica",3.9,39918),</v>
+        <v>("The Practical Progressive: How to Build a Twenty-first Century Political Movement","Payne, Erica",3.9,39918),</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5861,7 +5866,7 @@
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>The Purpose Driven Life: What on Earth Am I Here for?","Warren, Rick",3.87,39979),</v>
+        <v>("The Purpose Driven Life: What on Earth Am I Here for?","Warren, Rick",3.87,39979),</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5894,7 +5899,7 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>The White Man's Burden: Why the West's Efforts to Aid the Rest Have Done So Much Ill and So Little Good","Easterly, William",3.82,39563),</v>
+        <v>("The White Man's Burden: Why the West's Efforts to Aid the Rest Have Done So Much Ill and So Little Good","Easterly, William",3.82,39563),</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5927,7 +5932,7 @@
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>This Is Cuba: An Outlaw Culture Survives","Corbett, Ben",3.7,39590),</v>
+        <v>("This Is Cuba: An Outlaw Culture Survives","Corbett, Ben",3.7,39590),</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5960,7 +5965,7 @@
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>Up Against the Wall: Violence in the Making and Unmaking of the Black Panther Party","Austin, Curtis J.",4.16,39976),</v>
+        <v>("Up Against the Wall: Violence in the Making and Unmaking of the Black Panther Party","Austin, Curtis J.",4.16,39976),</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5993,7 +5998,7 @@
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>War and the Soul: Healing Our Nation's Veterans from Post-traumatic Stress Disorder","Tick, Edward",4.34,39637),</v>
+        <v>("War and the Soul: Healing Our Nation's Veterans from Post-traumatic Stress Disorder","Tick, Edward",4.34,39637),</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6026,7 +6031,7 @@
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>Writing Down the Bones: Freeing the Writer Within","Goldberg, Natalie",4.17,39445),</v>
+        <v>("Writing Down the Bones: Freeing the Writer Within","Goldberg, Natalie",4.17,39445),</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6061,8 +6066,8 @@
         <v>83</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" ref="J34:J45" si="1">CONCATENATE(B34,C34,D34,E34,F34,G34,H34,I34)</f>
-        <v>Built to Last: Successful Habits of Visionary Companies","Collins, James C.",3.95,39766),</v>
+        <f t="shared" ref="J34:J45" si="1">CONCATENATE(A34, B34,C34,D34,E34,F34,G34,H34,I34)</f>
+        <v>("Built to Last: Successful Habits of Visionary Companies","Collins, James C.",3.95,39766),</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6095,7 +6100,7 @@
       </c>
       <c r="J35" t="str">
         <f t="shared" si="1"/>
-        <v>Extremely Loud and Incredibly Close","Safran Foer, Jonathan",3.97,39445),</v>
+        <v>("Extremely Loud and Incredibly Close","Safran Foer, Jonathan",3.97,39445),</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6128,7 +6133,7 @@
       </c>
       <c r="J36" t="str">
         <f t="shared" si="1"/>
-        <v>Full Frontal Feminism","Valenti, Jessica *",3.85,39453),</v>
+        <v>("Full Frontal Feminism","Valenti, Jessica *",3.85,39453),</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6161,7 +6166,7 @@
       </c>
       <c r="J37" t="str">
         <f t="shared" si="1"/>
-        <v>Games for Actors and Non-Actors","Boal, Augusto",4.35,39453),</v>
+        <v>("Games for Actors and Non-Actors","Boal, Augusto",4.35,39453),</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6194,7 +6199,7 @@
       </c>
       <c r="J38" t="str">
         <f t="shared" si="1"/>
-        <v>Here Comes Everybody: The Power of Organizing Without Organizations","Shirky, Clay",3.82,39959),</v>
+        <v>("Here Comes Everybody: The Power of Organizing Without Organizations","Shirky, Clay",3.82,39959),</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6227,7 +6232,7 @@
       </c>
       <c r="J39" t="str">
         <f t="shared" si="1"/>
-        <v>Lying Awake","Salzman, Mark",3.8,39603),</v>
+        <v>("Lying Awake","Salzman, Mark",3.8,39603),</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6260,7 +6265,7 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="1"/>
-        <v>Mountains Beyond Mountains: The Quest of Dr. Paul Farmer, A Man Who Would Cure the World","Kidder, Tracy",4.2,39489),</v>
+        <v>("Mountains Beyond Mountains: The Quest of Dr. Paul Farmer, A Man Who Would Cure the World","Kidder, Tracy",4.2,39489),</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6293,7 +6298,7 @@
       </c>
       <c r="J41" t="str">
         <f t="shared" si="1"/>
-        <v>No Country For Old Men","McCarthy, Cormac",4.12,39467),</v>
+        <v>("No Country For Old Men","McCarthy, Cormac",4.12,39467),</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6326,7 +6331,7 @@
       </c>
       <c r="J42" t="str">
         <f t="shared" si="1"/>
-        <v>Oh Pure and Radiant Heart","Millet, Lydia",3.67,39489),</v>
+        <v>("Oh Pure and Radiant Heart","Millet, Lydia",3.67,39489),</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6359,7 +6364,7 @@
       </c>
       <c r="J43" t="str">
         <f t="shared" si="1"/>
-        <v>Predictably Irrational: The Hidden Forces That Shape Our Decisions","Ariely, Dan",4.08,39973),</v>
+        <v>("Predictably Irrational: The Hidden Forces That Shape Our Decisions","Ariely, Dan",4.08,39973),</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6392,7 +6397,7 @@
       </c>
       <c r="J44" t="str">
         <f t="shared" si="1"/>
-        <v>Ten Little Indians","Alexie, Sherman",4.08,39392),</v>
+        <v>("Ten Little Indians","Alexie, Sherman",4.08,39392),</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6425,7 +6430,7 @@
       </c>
       <c r="J45" t="str">
         <f t="shared" si="1"/>
-        <v>The Audacity of Hope: Thoughts on Reclaiming the American Dream","Obama, Barack",3.67,39542),</v>
+        <v>("The Audacity of Hope: Thoughts on Reclaiming the American Dream","Obama, Barack",3.67,39542),</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>